<commit_message>
added lane 29a (Ponatilink libraries Region 3 D0)
</commit_message>
<xml_diff>
--- a/data/Consensus_Data/Libraries_informatics_progress_sheet.xlsx
+++ b/data/Consensus_Data/Libraries_informatics_progress_sheet.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/hzi14_psu_edu/Documents/RProjects/duplex_sequencing_screen/data/Consensus_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A53EAE12-F6DD-E840-89F1-5D6C4362DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ECB55D39-8F77-DD43-867D-6BCD4AE6B5FC}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{A53EAE12-F6DD-E840-89F1-5D6C4362DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BB4B5FF-59DC-3D4B-A81C-8D85319C37AB}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{56B4F61F-FF81-5047-AAC1-D1034B21E8E5}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29920" windowHeight="18680" activeTab="2" xr2:uid="{56B4F61F-FF81-5047-AAC1-D1034B21E8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Lane29" sheetId="1" r:id="rId1"/>
     <sheet name="Lane28" sheetId="2" r:id="rId2"/>
+    <sheet name="Lane29c" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="473" uniqueCount="110">
   <si>
     <t>Lane</t>
   </si>
@@ -285,14 +286,103 @@
   </si>
   <si>
     <t>Partial consensus calling done</t>
+  </si>
+  <si>
+    <t>lowsequencingdepth</t>
+  </si>
+  <si>
+    <t>This is data that was sequenced with novogene</t>
+  </si>
+  <si>
+    <t>This is data that was sequenced with Cheryl</t>
+  </si>
+  <si>
+    <t>7 days completion time, with MAFFT aligner</t>
+  </si>
+  <si>
+    <t>29c</t>
+  </si>
+  <si>
+    <t>sample1_Ivan_L1_D6</t>
+  </si>
+  <si>
+    <t>sample2_Ivan_L2_D6</t>
+  </si>
+  <si>
+    <t>sample3_Ivan_L1_D8</t>
+  </si>
+  <si>
+    <t>sample4_Ivan_L2_D8</t>
+  </si>
+  <si>
+    <t>sample5_LTK_R1_D0</t>
+  </si>
+  <si>
+    <t>sample6_LTK_R1_ND_D6_A</t>
+  </si>
+  <si>
+    <t>sample7_LTK_R1_ND_D6_B</t>
+  </si>
+  <si>
+    <t>sample8_LTK_R1_Lor_D6_A</t>
+  </si>
+  <si>
+    <t>sample9_LTK_R1_Lor_D6_B</t>
+  </si>
+  <si>
+    <t>sample10_LTK_R1_Zot_D6_A</t>
+  </si>
+  <si>
+    <t>sample11_LTK_R1_Zot_D6_B</t>
+  </si>
+  <si>
+    <t>sample12_LTK_R2_D0</t>
+  </si>
+  <si>
+    <t>sample13_LTK_R2_ND_D6_A</t>
+  </si>
+  <si>
+    <t>sample14_LTK_R2_ND_D6_B</t>
+  </si>
+  <si>
+    <t>sample15_LTK_R2_Lor_D6_A</t>
+  </si>
+  <si>
+    <t>sample16_LTK_R2_Lor_D6_B</t>
+  </si>
+  <si>
+    <t>sample17_LTK_R2_Zot_D6_A</t>
+  </si>
+  <si>
+    <t>sample18_LTK_R2_Zot_D6_B</t>
+  </si>
+  <si>
+    <t>sample19_Veri_L1_D0</t>
+  </si>
+  <si>
+    <t>sample20_Veri_L2_D0</t>
+  </si>
+  <si>
+    <t>sample21_Veri_L1_D14</t>
+  </si>
+  <si>
+    <t>sample22_Veri_L2_D14</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -333,15 +423,36 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -694,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA62B7D-73D1-E341-9DF1-4F7931EE4048}">
   <dimension ref="A1:G33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,10 +1030,16 @@
         <v>33</v>
       </c>
       <c r="D12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>86</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -1032,6 +1149,9 @@
       <c r="E18" t="s">
         <v>6</v>
       </c>
+      <c r="G18" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
@@ -1108,7 +1228,7 @@
       <c r="B23">
         <v>1</v>
       </c>
-      <c r="C23" s="1" t="s">
+      <c r="C23" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D23" t="s">
@@ -1118,10 +1238,10 @@
         <v>6</v>
       </c>
       <c r="F23" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="G23" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -1131,7 +1251,7 @@
       <c r="B24">
         <v>2</v>
       </c>
-      <c r="C24" s="1" t="s">
+      <c r="C24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D24" t="s">
@@ -1141,10 +1261,10 @@
         <v>6</v>
       </c>
       <c r="F24" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="G24" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -1154,20 +1274,20 @@
       <c r="B25">
         <v>3</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="C25" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E25" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F25" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
       <c r="G25" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -1177,7 +1297,7 @@
       <c r="B26">
         <v>4</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C26" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D26" t="s">
@@ -1187,7 +1307,7 @@
         <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -1197,7 +1317,7 @@
       <c r="B27">
         <v>5</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C27" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D27" t="s">
@@ -1207,7 +1327,7 @@
         <v>6</v>
       </c>
       <c r="F27" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -1217,17 +1337,17 @@
       <c r="B28">
         <v>6</v>
       </c>
-      <c r="C28" s="1" t="s">
+      <c r="C28" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F28" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -1237,7 +1357,7 @@
       <c r="B29">
         <v>7</v>
       </c>
-      <c r="C29" s="1" t="s">
+      <c r="C29" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D29" t="s">
@@ -1247,7 +1367,7 @@
         <v>7</v>
       </c>
       <c r="F29" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -1257,17 +1377,17 @@
       <c r="B30">
         <v>8</v>
       </c>
-      <c r="C30" s="1" t="s">
+      <c r="C30" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E30" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F30" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -1277,17 +1397,17 @@
       <c r="B31">
         <v>9</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="C31" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E31" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F31" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -1297,7 +1417,7 @@
       <c r="B32">
         <v>10</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="C32" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D32" t="s">
@@ -1307,7 +1427,7 @@
         <v>6</v>
       </c>
       <c r="F32" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
@@ -1317,7 +1437,7 @@
       <c r="B33">
         <v>11</v>
       </c>
-      <c r="C33" s="1" t="s">
+      <c r="C33" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D33" t="s">
@@ -1327,12 +1447,13 @@
         <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>11</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="D2:E200 F23:F33 G23:G25">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="N">
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D2:E200 F23:F33 G23:G25 F12">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1342,66 +1463,1206 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F2D043-530F-0C4F-9959-B35E9CE1CB91}">
-  <dimension ref="A1:G39"/>
+  <dimension ref="A1:G63"/>
   <sheetViews>
     <sheetView zoomScale="144" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="D1" sqref="D1:E39"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="8.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>28</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
+      <c r="E2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>28</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>28</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>28</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>7</v>
+      </c>
+      <c r="E6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F6" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>28</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F7" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>51</v>
+      </c>
+      <c r="D8" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>28</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+      <c r="E9" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>28</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>53</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+      <c r="F10" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>28</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>28</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+      <c r="F12" t="s">
+        <v>76</v>
+      </c>
+      <c r="G12" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>28</v>
+      </c>
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E13" t="s">
+        <v>6</v>
+      </c>
+      <c r="F13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>28</v>
+      </c>
+      <c r="B14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" t="s">
+        <v>6</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
+      </c>
+      <c r="F14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>28</v>
+      </c>
+      <c r="B15">
+        <v>14</v>
+      </c>
+      <c r="C15" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+      <c r="F15" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>28</v>
+      </c>
+      <c r="B16">
+        <v>15</v>
+      </c>
+      <c r="C16" t="s">
+        <v>59</v>
+      </c>
+      <c r="D16" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" t="s">
+        <v>6</v>
+      </c>
+      <c r="F16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>28</v>
+      </c>
+      <c r="B17">
+        <v>16</v>
+      </c>
+      <c r="C17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D17" t="s">
+        <v>6</v>
+      </c>
+      <c r="E17" t="s">
+        <v>6</v>
+      </c>
+      <c r="F17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>28</v>
+      </c>
+      <c r="B18">
+        <v>17</v>
+      </c>
+      <c r="C18" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>28</v>
+      </c>
+      <c r="B19">
+        <v>18</v>
+      </c>
+      <c r="C19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D19" t="s">
+        <v>6</v>
+      </c>
+      <c r="E19" t="s">
+        <v>6</v>
+      </c>
+      <c r="F19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>28</v>
+      </c>
+      <c r="B20">
+        <v>19</v>
+      </c>
+      <c r="C20" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" t="s">
+        <v>6</v>
+      </c>
+      <c r="E20" t="s">
+        <v>6</v>
+      </c>
+      <c r="F20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>20</v>
+      </c>
+      <c r="C21" t="s">
+        <v>64</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>28</v>
+      </c>
+      <c r="B22">
+        <v>21</v>
+      </c>
+      <c r="C22" t="s">
+        <v>65</v>
+      </c>
+      <c r="D22" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>28</v>
+      </c>
+      <c r="B23">
+        <v>22</v>
+      </c>
+      <c r="C23" t="s">
+        <v>66</v>
+      </c>
+      <c r="D23" t="s">
+        <v>6</v>
+      </c>
+      <c r="E23" t="s">
+        <v>6</v>
+      </c>
+      <c r="F23" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>28</v>
+      </c>
+      <c r="B24">
+        <v>23</v>
+      </c>
+      <c r="C24" t="s">
+        <v>67</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>28</v>
+      </c>
+      <c r="B25">
+        <v>24</v>
+      </c>
+      <c r="C25" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>6</v>
+      </c>
+      <c r="E25" t="s">
+        <v>6</v>
+      </c>
+      <c r="F25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>69</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>45</v>
+      </c>
+      <c r="D26" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" t="s">
+        <v>7</v>
+      </c>
+      <c r="F26" t="s">
+        <v>76</v>
+      </c>
+      <c r="G26" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>69</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>45</v>
+      </c>
+      <c r="D27" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" t="s">
+        <v>7</v>
+      </c>
+      <c r="F27" t="s">
+        <v>76</v>
+      </c>
+      <c r="G27" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>69</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>73</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+      <c r="F28" t="s">
+        <v>76</v>
+      </c>
+      <c r="G28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>69</v>
+      </c>
+      <c r="B29">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" t="s">
+        <v>6</v>
+      </c>
+      <c r="E29" t="s">
+        <v>7</v>
+      </c>
+      <c r="F29" t="s">
+        <v>76</v>
+      </c>
+      <c r="G29" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30">
+        <v>5</v>
+      </c>
+      <c r="C30" t="s">
+        <v>53</v>
+      </c>
+      <c r="D30" t="s">
+        <v>7</v>
+      </c>
+      <c r="E30" t="s">
+        <v>7</v>
+      </c>
+      <c r="F30" t="s">
+        <v>76</v>
+      </c>
+      <c r="G30" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B31">
+        <v>6</v>
+      </c>
+      <c r="C31" t="s">
+        <v>53</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+      <c r="F31" t="s">
+        <v>76</v>
+      </c>
+      <c r="G31" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32">
+        <v>7</v>
+      </c>
+      <c r="C32" t="s">
+        <v>74</v>
+      </c>
+      <c r="D32" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" t="s">
+        <v>7</v>
+      </c>
+      <c r="F32" t="s">
+        <v>76</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33">
+        <v>8</v>
+      </c>
+      <c r="C33" t="s">
+        <v>74</v>
+      </c>
+      <c r="D33" t="s">
+        <v>7</v>
+      </c>
+      <c r="E33" t="s">
+        <v>7</v>
+      </c>
+      <c r="F33" t="s">
+        <v>76</v>
+      </c>
+      <c r="G33" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B34">
+        <v>9</v>
+      </c>
+      <c r="C34" t="s">
+        <v>61</v>
+      </c>
+      <c r="D34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>69</v>
+      </c>
+      <c r="B35">
+        <v>10</v>
+      </c>
+      <c r="C35" t="s">
+        <v>61</v>
+      </c>
+      <c r="D35" t="s">
+        <v>6</v>
+      </c>
+      <c r="E35" t="s">
+        <v>6</v>
+      </c>
+      <c r="F35" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>69</v>
+      </c>
+      <c r="B36">
+        <v>11</v>
+      </c>
+      <c r="C36" t="s">
+        <v>75</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+      <c r="F36" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>69</v>
+      </c>
+      <c r="B37">
+        <v>12</v>
+      </c>
+      <c r="C37" t="s">
+        <v>75</v>
+      </c>
+      <c r="D37" t="s">
+        <v>6</v>
+      </c>
+      <c r="E37" t="s">
+        <v>6</v>
+      </c>
+      <c r="F37" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38">
+        <v>13</v>
+      </c>
+      <c r="C38" t="s">
+        <v>71</v>
+      </c>
+      <c r="D38" t="s">
+        <v>6</v>
+      </c>
+      <c r="E38" t="s">
+        <v>6</v>
+      </c>
+      <c r="F38" t="s">
+        <v>76</v>
+      </c>
+      <c r="G38" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>69</v>
+      </c>
+      <c r="B39">
+        <v>14</v>
+      </c>
+      <c r="C39" t="s">
+        <v>72</v>
+      </c>
+      <c r="D39" t="s">
+        <v>6</v>
+      </c>
+      <c r="E39" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" t="s">
+        <v>76</v>
+      </c>
+      <c r="G39" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40">
+        <v>28</v>
+      </c>
+      <c r="B40">
+        <v>1</v>
+      </c>
+      <c r="C40" t="s">
+        <v>45</v>
+      </c>
+      <c r="G40" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>28</v>
+      </c>
+      <c r="B41">
+        <v>2</v>
+      </c>
+      <c r="C41" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>28</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>28</v>
+      </c>
+      <c r="B43">
+        <v>4</v>
+      </c>
+      <c r="C43" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>28</v>
+      </c>
+      <c r="B44">
+        <v>5</v>
+      </c>
+      <c r="C44" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>28</v>
+      </c>
+      <c r="B45">
+        <v>6</v>
+      </c>
+      <c r="C45" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>28</v>
+      </c>
+      <c r="B46">
+        <v>7</v>
+      </c>
+      <c r="C46" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>28</v>
+      </c>
+      <c r="B47">
+        <v>8</v>
+      </c>
+      <c r="C47" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>28</v>
+      </c>
+      <c r="B48">
+        <v>9</v>
+      </c>
+      <c r="C48" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>28</v>
+      </c>
+      <c r="B49">
+        <v>10</v>
+      </c>
+      <c r="C49" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>28</v>
+      </c>
+      <c r="B50">
+        <v>11</v>
+      </c>
+      <c r="C50" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>28</v>
+      </c>
+      <c r="B51">
+        <v>12</v>
+      </c>
+      <c r="C51" t="s">
+        <v>56</v>
+      </c>
+      <c r="D51" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>28</v>
+      </c>
+      <c r="B52">
+        <v>13</v>
+      </c>
+      <c r="C52" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>28</v>
+      </c>
+      <c r="B53">
+        <v>14</v>
+      </c>
+      <c r="C53" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A54">
+        <v>28</v>
+      </c>
+      <c r="B54">
+        <v>15</v>
+      </c>
+      <c r="C54" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A55">
+        <v>28</v>
+      </c>
+      <c r="B55">
+        <v>16</v>
+      </c>
+      <c r="C55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A56">
+        <v>28</v>
+      </c>
+      <c r="B56">
+        <v>17</v>
+      </c>
+      <c r="C56" t="s">
+        <v>61</v>
+      </c>
+      <c r="D56" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A57">
+        <v>28</v>
+      </c>
+      <c r="B57">
+        <v>18</v>
+      </c>
+      <c r="C57" t="s">
+        <v>62</v>
+      </c>
+      <c r="D57" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>28</v>
+      </c>
+      <c r="B58">
+        <v>19</v>
+      </c>
+      <c r="C58" t="s">
+        <v>63</v>
+      </c>
+      <c r="D58" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A59">
+        <v>28</v>
+      </c>
+      <c r="B59">
+        <v>20</v>
+      </c>
+      <c r="C59" t="s">
+        <v>64</v>
+      </c>
+      <c r="D59" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A60">
+        <v>28</v>
+      </c>
+      <c r="B60">
+        <v>21</v>
+      </c>
+      <c r="C60" t="s">
+        <v>65</v>
+      </c>
+      <c r="D60" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A61">
+        <v>28</v>
+      </c>
+      <c r="B61">
+        <v>22</v>
+      </c>
+      <c r="C61" t="s">
+        <v>66</v>
+      </c>
+      <c r="D61" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A62">
+        <v>28</v>
+      </c>
+      <c r="B62">
+        <v>23</v>
+      </c>
+      <c r="C62" t="s">
+        <v>67</v>
+      </c>
+      <c r="D62" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A63">
+        <v>28</v>
+      </c>
+      <c r="B63">
+        <v>24</v>
+      </c>
+      <c r="C63" t="s">
+        <v>68</v>
+      </c>
+      <c r="D63" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="D2:E33 F2:F25 G12">
+    <cfRule type="containsText" dxfId="4" priority="2" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",D2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G38:G39">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",G38)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1375D86A-AC32-1C40-AB96-8DC0895D6135}">
+  <dimension ref="A1:G23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2">
-        <v>28</v>
+      <c r="A2" t="s">
+        <v>87</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>45</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="F2" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3">
-        <v>28</v>
+      <c r="A3" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>46</v>
+        <v>89</v>
       </c>
       <c r="D3" t="s">
         <v>7</v>
@@ -1409,19 +2670,16 @@
       <c r="E3" t="s">
         <v>7</v>
       </c>
-      <c r="F3" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4">
-        <v>28</v>
+      <c r="A4" t="s">
+        <v>87</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>47</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1429,19 +2687,16 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5">
-        <v>28</v>
+      <c r="A5" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>48</v>
+        <v>91</v>
       </c>
       <c r="D5" t="s">
         <v>7</v>
@@ -1449,19 +2704,16 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="F5" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6">
-        <v>28</v>
+      <c r="A6" t="s">
+        <v>87</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>92</v>
       </c>
       <c r="D6" t="s">
         <v>7</v>
@@ -1469,19 +2721,16 @@
       <c r="E6" t="s">
         <v>7</v>
       </c>
-      <c r="F6" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7">
-        <v>28</v>
+      <c r="A7" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="D7" t="s">
         <v>7</v>
@@ -1489,39 +2738,33 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8">
-        <v>28</v>
+      <c r="A8" t="s">
+        <v>87</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>51</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E8" t="s">
         <v>7</v>
       </c>
-      <c r="F8" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9">
-        <v>28</v>
+      <c r="A9" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>52</v>
+        <v>95</v>
       </c>
       <c r="D9" t="s">
         <v>7</v>
@@ -1529,19 +2772,16 @@
       <c r="E9" t="s">
         <v>7</v>
       </c>
-      <c r="F9" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10">
-        <v>28</v>
+      <c r="A10" t="s">
+        <v>87</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>53</v>
+        <v>96</v>
       </c>
       <c r="D10" t="s">
         <v>7</v>
@@ -1549,626 +2789,235 @@
       <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11">
-        <v>28</v>
+      <c r="A11" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>97</v>
       </c>
       <c r="D11" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E11" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12">
-        <v>28</v>
+      <c r="A12" t="s">
+        <v>87</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>55</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E12" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" t="s">
-        <v>76</v>
-      </c>
-      <c r="G12" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13">
-        <v>28</v>
+      <c r="A13" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="D13" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E13" t="s">
-        <v>6</v>
-      </c>
-      <c r="F13" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14">
-        <v>28</v>
+      <c r="A14" t="s">
+        <v>87</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>57</v>
+        <v>100</v>
       </c>
       <c r="D14" t="s">
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>6</v>
-      </c>
-      <c r="F14" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15">
-        <v>28</v>
+      <c r="A15" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>58</v>
+        <v>101</v>
       </c>
       <c r="D15" t="s">
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>6</v>
-      </c>
-      <c r="F15" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16">
-        <v>28</v>
+      <c r="A16" t="s">
+        <v>87</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>59</v>
+        <v>102</v>
       </c>
       <c r="D16" t="s">
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>6</v>
-      </c>
-      <c r="F16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17">
-        <v>28</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>103</v>
       </c>
       <c r="D17" t="s">
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>6</v>
-      </c>
-      <c r="F17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18">
-        <v>28</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" t="s">
+        <v>87</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>61</v>
+        <v>104</v>
       </c>
       <c r="D18" t="s">
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>6</v>
-      </c>
-      <c r="F18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A19">
-        <v>28</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>62</v>
+        <v>105</v>
       </c>
       <c r="D19" t="s">
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>6</v>
-      </c>
-      <c r="F19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A20">
-        <v>28</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>87</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="D20" t="s">
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>6</v>
-      </c>
-      <c r="F20" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A21">
-        <v>28</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>64</v>
+        <v>107</v>
       </c>
       <c r="D21" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E21" t="s">
-        <v>6</v>
-      </c>
-      <c r="F21" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A22">
-        <v>28</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>87</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>65</v>
+        <v>108</v>
       </c>
       <c r="D22" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F22" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A23">
-        <v>28</v>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>87</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>66</v>
+        <v>109</v>
       </c>
       <c r="D23" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E23" t="s">
-        <v>6</v>
-      </c>
-      <c r="F23" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A24">
-        <v>28</v>
-      </c>
-      <c r="B24">
-        <v>23</v>
-      </c>
-      <c r="C24" t="s">
-        <v>67</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" t="s">
-        <v>6</v>
-      </c>
-      <c r="F24" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A25">
-        <v>28</v>
-      </c>
-      <c r="B25">
-        <v>24</v>
-      </c>
-      <c r="C25" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>69</v>
-      </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>45</v>
-      </c>
-      <c r="D26" t="s">
-        <v>6</v>
-      </c>
-      <c r="E26" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" t="s">
-        <v>76</v>
-      </c>
-      <c r="G26" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-      <c r="B27">
-        <v>2</v>
-      </c>
-      <c r="C27" t="s">
-        <v>45</v>
-      </c>
-      <c r="D27" t="s">
-        <v>7</v>
-      </c>
-      <c r="E27" t="s">
-        <v>7</v>
-      </c>
-      <c r="F27" t="s">
-        <v>76</v>
-      </c>
-      <c r="G27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>69</v>
-      </c>
-      <c r="B28">
-        <v>3</v>
-      </c>
-      <c r="C28" t="s">
-        <v>73</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-      <c r="E28" t="s">
-        <v>7</v>
-      </c>
-      <c r="F28" t="s">
-        <v>76</v>
-      </c>
-      <c r="G28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>69</v>
-      </c>
-      <c r="B29">
-        <v>4</v>
-      </c>
-      <c r="C29" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" t="s">
-        <v>7</v>
-      </c>
-      <c r="F29" t="s">
-        <v>76</v>
-      </c>
-      <c r="G29" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>69</v>
-      </c>
-      <c r="B30">
-        <v>5</v>
-      </c>
-      <c r="C30" t="s">
-        <v>53</v>
-      </c>
-      <c r="D30" t="s">
-        <v>7</v>
-      </c>
-      <c r="E30" t="s">
-        <v>7</v>
-      </c>
-      <c r="F30" t="s">
-        <v>76</v>
-      </c>
-      <c r="G30" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>69</v>
-      </c>
-      <c r="B31">
-        <v>6</v>
-      </c>
-      <c r="C31" t="s">
-        <v>53</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-      <c r="E31" t="s">
-        <v>7</v>
-      </c>
-      <c r="F31" t="s">
-        <v>76</v>
-      </c>
-      <c r="G31" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>69</v>
-      </c>
-      <c r="B32">
-        <v>7</v>
-      </c>
-      <c r="C32" t="s">
-        <v>74</v>
-      </c>
-      <c r="D32" t="s">
-        <v>7</v>
-      </c>
-      <c r="E32" t="s">
-        <v>7</v>
-      </c>
-      <c r="F32" t="s">
-        <v>76</v>
-      </c>
-      <c r="G32" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33">
-        <v>8</v>
-      </c>
-      <c r="C33" t="s">
-        <v>74</v>
-      </c>
-      <c r="D33" t="s">
-        <v>7</v>
-      </c>
-      <c r="E33" t="s">
-        <v>7</v>
-      </c>
-      <c r="F33" t="s">
-        <v>76</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34">
-        <v>9</v>
-      </c>
-      <c r="C34" t="s">
-        <v>61</v>
-      </c>
-      <c r="D34" t="s">
-        <v>6</v>
-      </c>
-      <c r="E34" t="s">
-        <v>6</v>
-      </c>
-      <c r="F34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>69</v>
-      </c>
-      <c r="B35">
-        <v>10</v>
-      </c>
-      <c r="C35" t="s">
-        <v>61</v>
-      </c>
-      <c r="D35" t="s">
-        <v>6</v>
-      </c>
-      <c r="E35" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>69</v>
-      </c>
-      <c r="B36">
-        <v>11</v>
-      </c>
-      <c r="C36" t="s">
-        <v>75</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-      <c r="E36" t="s">
-        <v>6</v>
-      </c>
-      <c r="F36" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>69</v>
-      </c>
-      <c r="B37">
-        <v>12</v>
-      </c>
-      <c r="C37" t="s">
-        <v>75</v>
-      </c>
-      <c r="D37" t="s">
-        <v>6</v>
-      </c>
-      <c r="E37" t="s">
-        <v>6</v>
-      </c>
-      <c r="F37" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>69</v>
-      </c>
-      <c r="B38">
-        <v>13</v>
-      </c>
-      <c r="C38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D38" t="s">
-        <v>6</v>
-      </c>
-      <c r="E38" t="s">
-        <v>6</v>
-      </c>
-      <c r="F38" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>69</v>
-      </c>
-      <c r="B39">
-        <v>14</v>
-      </c>
-      <c r="C39" t="s">
-        <v>72</v>
-      </c>
-      <c r="D39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E39" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="D2:E33 F2:F25 G12">
-    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="N">
+  <conditionalFormatting sqref="D2:E33">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Added a bug fix to merge_samples.R and updated imatinib heatmaps
</commit_message>
<xml_diff>
--- a/data/Consensus_Data/Libraries_informatics_progress_sheet.xlsx
+++ b/data/Consensus_Data/Libraries_informatics_progress_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pennstateoffice365-my.sharepoint.com/personal/hzi14_psu_edu/Documents/RProjects/duplex_sequencing_screen/data/Consensus_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="30" documentId="8_{A53EAE12-F6DD-E840-89F1-5D6C4362DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{74D8FE72-0753-E74E-8F2E-057907C82E9F}"/>
+  <xr:revisionPtr revIDLastSave="68" documentId="8_{A53EAE12-F6DD-E840-89F1-5D6C4362DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{878594EE-211F-AB42-AB82-8FE1D274633C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{56B4F61F-FF81-5047-AAC1-D1034B21E8E5}"/>
+    <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{56B4F61F-FF81-5047-AAC1-D1034B21E8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Lane28" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="561" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="627" uniqueCount="135">
   <si>
     <t>Lane</t>
   </si>
@@ -372,7 +372,7 @@
     <t>R5a 1</t>
   </si>
   <si>
-    <t>R5a1</t>
+    <t>R5a3</t>
   </si>
   <si>
     <t>almost</t>
@@ -415,6 +415,33 @@
   </si>
   <si>
     <t>30.4M</t>
+  </si>
+  <si>
+    <t>Partial consensus of combined samples from original + resequencing samples</t>
+  </si>
+  <si>
+    <t>1_2</t>
+  </si>
+  <si>
+    <t>3_4</t>
+  </si>
+  <si>
+    <t>5_6</t>
+  </si>
+  <si>
+    <t>7_8</t>
+  </si>
+  <si>
+    <t>9_10</t>
+  </si>
+  <si>
+    <t>11_12</t>
+  </si>
+  <si>
+    <t>Completed consensus of combined samples from original + resequencing samples</t>
+  </si>
+  <si>
+    <t>28b</t>
   </si>
 </sst>
 </file>
@@ -500,7 +527,17 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="16">
+  <dxfs count="17">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -971,16 +1008,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F2D043-530F-0C4F-9959-B35E9CE1CB91}">
-  <dimension ref="A1:J63"/>
+  <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="200" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" customWidth="1"/>
     <col min="3" max="3" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.1640625" customWidth="1"/>
+    <col min="5" max="5" width="13.33203125" customWidth="1"/>
     <col min="10" max="10" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1672,7 +1711,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>69</v>
       </c>
@@ -1695,7 +1734,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -1715,7 +1754,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>69</v>
       </c>
@@ -1735,7 +1774,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>69</v>
       </c>
@@ -1755,7 +1794,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>69</v>
       </c>
@@ -1775,18 +1814,18 @@
         <v>76</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>69</v>
       </c>
-      <c r="B38">
-        <v>13</v>
+      <c r="B38" t="s">
+        <v>127</v>
       </c>
       <c r="C38" t="s">
-        <v>71</v>
+        <v>45</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E38" t="s">
         <v>6</v>
@@ -1795,21 +1834,21 @@
         <v>76</v>
       </c>
       <c r="G38" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.2">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>69</v>
       </c>
-      <c r="B39">
-        <v>14</v>
+      <c r="B39" t="s">
+        <v>128</v>
       </c>
       <c r="C39" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D39" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="E39" t="s">
         <v>6</v>
@@ -1818,123 +1857,156 @@
         <v>76</v>
       </c>
       <c r="G39" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>69</v>
+      </c>
+      <c r="B40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C40" t="s">
+        <v>53</v>
+      </c>
+      <c r="D40" t="s">
+        <v>7</v>
+      </c>
+      <c r="E40" t="s">
+        <v>6</v>
+      </c>
+      <c r="F40" t="s">
+        <v>76</v>
+      </c>
+      <c r="G40" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B41" t="s">
+        <v>130</v>
+      </c>
+      <c r="C41" t="s">
+        <v>74</v>
+      </c>
+      <c r="D41" t="s">
+        <v>6</v>
+      </c>
+      <c r="E41" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" t="s">
+        <v>76</v>
+      </c>
+      <c r="G41" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>69</v>
+      </c>
+      <c r="B42" t="s">
+        <v>131</v>
+      </c>
+      <c r="C42" t="s">
+        <v>61</v>
+      </c>
+      <c r="D42" t="s">
+        <v>6</v>
+      </c>
+      <c r="E42" t="s">
+        <v>6</v>
+      </c>
+      <c r="F42" t="s">
+        <v>76</v>
+      </c>
+      <c r="G42" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>69</v>
+      </c>
+      <c r="B43" t="s">
+        <v>132</v>
+      </c>
+      <c r="C43" t="s">
+        <v>75</v>
+      </c>
+      <c r="D43" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" t="s">
+        <v>76</v>
+      </c>
+      <c r="G43" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44">
+        <v>13</v>
+      </c>
+      <c r="C44" t="s">
+        <v>71</v>
+      </c>
+      <c r="D44" t="s">
+        <v>6</v>
+      </c>
+      <c r="E44" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G44" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A40">
-        <v>28</v>
-      </c>
-      <c r="B40">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>69</v>
+      </c>
+      <c r="B45">
+        <v>14</v>
+      </c>
+      <c r="C45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="E45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>76</v>
+      </c>
+      <c r="G45" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46">
         <v>1</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C46" t="s">
         <v>45</v>
-      </c>
-      <c r="D40" t="s">
-        <v>7</v>
-      </c>
-      <c r="F40" t="s">
-        <v>111</v>
-      </c>
-      <c r="G40" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A41">
-        <v>28</v>
-      </c>
-      <c r="B41">
-        <v>2</v>
-      </c>
-      <c r="C41" t="s">
-        <v>46</v>
-      </c>
-      <c r="D41" t="s">
-        <v>7</v>
-      </c>
-      <c r="F41" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A42">
-        <v>28</v>
-      </c>
-      <c r="B42">
-        <v>3</v>
-      </c>
-      <c r="C42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A43">
-        <v>28</v>
-      </c>
-      <c r="B43">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>28</v>
-      </c>
-      <c r="B44">
-        <v>5</v>
-      </c>
-      <c r="C44" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>28</v>
-      </c>
-      <c r="B45">
-        <v>6</v>
-      </c>
-      <c r="C45" t="s">
-        <v>50</v>
-      </c>
-      <c r="D45" t="s">
-        <v>7</v>
-      </c>
-      <c r="F45" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A46">
-        <v>28</v>
-      </c>
-      <c r="B46">
-        <v>7</v>
-      </c>
-      <c r="C46" t="s">
-        <v>51</v>
       </c>
       <c r="D46" t="s">
         <v>7</v>
@@ -1942,16 +2014,19 @@
       <c r="F46" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A47">
-        <v>28</v>
+      <c r="G46" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>134</v>
       </c>
       <c r="B47">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="C47" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="D47" t="s">
         <v>7</v>
@@ -1959,21 +2034,16 @@
       <c r="F47" t="s">
         <v>111</v>
       </c>
-      <c r="H47" s="4"/>
-      <c r="I47" s="5" t="s">
-        <v>117</v>
-      </c>
-      <c r="J47" s="5"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A48">
-        <v>28</v>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>134</v>
       </c>
       <c r="B48">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="C48" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="D48" t="s">
         <v>7</v>
@@ -1981,138 +2051,106 @@
       <c r="F48" t="s">
         <v>111</v>
       </c>
-      <c r="H48" s="4"/>
-      <c r="I48" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="J48" s="4" t="s">
-        <v>114</v>
-      </c>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A49">
-        <v>28</v>
+      <c r="A49" t="s">
+        <v>134</v>
       </c>
       <c r="B49">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C49" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="D49" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F49" t="s">
         <v>111</v>
       </c>
-      <c r="H49" s="6" t="s">
-        <v>115</v>
-      </c>
-      <c r="I49" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="J49" s="4">
-        <v>826</v>
-      </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A50">
-        <v>28</v>
+      <c r="A50" t="s">
+        <v>134</v>
       </c>
       <c r="B50">
-        <v>11</v>
+        <v>5</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="D50" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F50" t="s">
         <v>111</v>
       </c>
-      <c r="H50" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="I50" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="J50" s="4">
-        <v>6922</v>
-      </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A51">
-        <v>28</v>
+      <c r="A51" t="s">
+        <v>134</v>
       </c>
       <c r="B51">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="C51" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="D51" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F51" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="52" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A52">
-        <v>28</v>
+      <c r="A52" t="s">
+        <v>134</v>
       </c>
       <c r="B52">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="C52" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="D52" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="F52" t="s">
         <v>111</v>
       </c>
-      <c r="H52" s="4"/>
-      <c r="I52" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="J52" s="5"/>
     </row>
     <row r="53" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A53">
-        <v>28</v>
+      <c r="A53" t="s">
+        <v>134</v>
       </c>
       <c r="B53">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C53" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="D53" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="F53" t="s">
         <v>111</v>
       </c>
       <c r="H53" s="4"/>
-      <c r="I53" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="J53" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="I53" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="J53" s="5"/>
     </row>
     <row r="54" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A54">
-        <v>28</v>
+      <c r="A54" t="s">
+        <v>134</v>
       </c>
       <c r="B54">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="C54" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="D54" t="s">
         <v>6</v>
@@ -2120,25 +2158,23 @@
       <c r="F54" t="s">
         <v>111</v>
       </c>
-      <c r="H54" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H54" s="4"/>
       <c r="I54" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="J54" s="4">
-        <v>1462</v>
+        <v>113</v>
+      </c>
+      <c r="J54" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A55">
-        <v>28</v>
+      <c r="A55" t="s">
+        <v>134</v>
       </c>
       <c r="B55">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="C55" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="D55" t="s">
         <v>6</v>
@@ -2147,24 +2183,24 @@
         <v>111</v>
       </c>
       <c r="H55" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I55" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J55" s="4">
-        <v>11500</v>
+        <v>826</v>
       </c>
     </row>
     <row r="56" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A56">
-        <v>28</v>
+      <c r="A56" t="s">
+        <v>134</v>
       </c>
       <c r="B56">
-        <v>17</v>
+        <v>11</v>
       </c>
       <c r="C56" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="D56" t="s">
         <v>6</v>
@@ -2172,16 +2208,25 @@
       <c r="F56" t="s">
         <v>111</v>
       </c>
+      <c r="H56" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I56" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="J56" s="4">
+        <v>6922</v>
+      </c>
     </row>
     <row r="57" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A57">
-        <v>28</v>
+      <c r="A57" t="s">
+        <v>134</v>
       </c>
       <c r="B57">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="D57" t="s">
         <v>6</v>
@@ -2189,21 +2234,16 @@
       <c r="F57" t="s">
         <v>111</v>
       </c>
-      <c r="H57" s="4"/>
-      <c r="I57" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="J57" s="5"/>
     </row>
     <row r="58" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A58">
-        <v>28</v>
+      <c r="A58" t="s">
+        <v>134</v>
       </c>
       <c r="B58">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C58" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="D58" t="s">
         <v>6</v>
@@ -2212,48 +2252,44 @@
         <v>111</v>
       </c>
       <c r="H58" s="4"/>
-      <c r="I58" s="4" t="s">
-        <v>113</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>114</v>
-      </c>
+      <c r="I58" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="J58" s="5"/>
     </row>
     <row r="59" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A59">
-        <v>28</v>
+      <c r="A59" t="s">
+        <v>134</v>
       </c>
       <c r="B59">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="C59" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D59" t="s">
-        <v>6</v>
+        <v>112</v>
       </c>
       <c r="F59" t="s">
         <v>111</v>
       </c>
-      <c r="H59" s="6" t="s">
-        <v>115</v>
-      </c>
+      <c r="H59" s="4"/>
       <c r="I59" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="J59" s="4">
-        <v>1161</v>
+        <v>113</v>
+      </c>
+      <c r="J59" s="4" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="60" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A60">
-        <v>28</v>
+      <c r="A60" t="s">
+        <v>134</v>
       </c>
       <c r="B60">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="D60" t="s">
         <v>6</v>
@@ -2262,24 +2298,24 @@
         <v>111</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="I60" s="4" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="J60" s="4">
-        <v>8555</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="61" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A61">
-        <v>28</v>
+      <c r="A61" t="s">
+        <v>134</v>
       </c>
       <c r="B61">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C61" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="D61" t="s">
         <v>6</v>
@@ -2287,16 +2323,25 @@
       <c r="F61" t="s">
         <v>111</v>
       </c>
+      <c r="H61" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I61" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="J61" s="4">
+        <v>11500</v>
+      </c>
     </row>
     <row r="62" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A62">
-        <v>28</v>
+      <c r="A62" t="s">
+        <v>134</v>
       </c>
       <c r="B62">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C62" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D62" t="s">
         <v>6</v>
@@ -2306,14 +2351,14 @@
       </c>
     </row>
     <row r="63" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A63">
-        <v>28</v>
+      <c r="A63" t="s">
+        <v>134</v>
       </c>
       <c r="B63">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="C63" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="D63" t="s">
         <v>6</v>
@@ -2321,67 +2366,204 @@
       <c r="F63" t="s">
         <v>111</v>
       </c>
+      <c r="H63" s="4"/>
+      <c r="I63" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A64" t="s">
+        <v>134</v>
+      </c>
+      <c r="B64">
+        <v>19</v>
+      </c>
+      <c r="C64" t="s">
+        <v>63</v>
+      </c>
+      <c r="D64" t="s">
+        <v>6</v>
+      </c>
+      <c r="F64" t="s">
+        <v>111</v>
+      </c>
+      <c r="H64" s="4"/>
+      <c r="I64" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="J64" s="4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A65" t="s">
+        <v>134</v>
+      </c>
+      <c r="B65">
+        <v>20</v>
+      </c>
+      <c r="C65" t="s">
+        <v>64</v>
+      </c>
+      <c r="D65" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" t="s">
+        <v>111</v>
+      </c>
+      <c r="H65" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="I65" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="J65" s="4">
+        <v>1161</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A66" t="s">
+        <v>134</v>
+      </c>
+      <c r="B66">
+        <v>21</v>
+      </c>
+      <c r="C66" t="s">
+        <v>65</v>
+      </c>
+      <c r="D66" t="s">
+        <v>6</v>
+      </c>
+      <c r="F66" t="s">
+        <v>111</v>
+      </c>
+      <c r="H66" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="I66" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="J66" s="4">
+        <v>8555</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A67" t="s">
+        <v>134</v>
+      </c>
+      <c r="B67">
+        <v>22</v>
+      </c>
+      <c r="C67" t="s">
+        <v>66</v>
+      </c>
+      <c r="D67" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A68" t="s">
+        <v>134</v>
+      </c>
+      <c r="B68">
+        <v>23</v>
+      </c>
+      <c r="C68" t="s">
+        <v>67</v>
+      </c>
+      <c r="D68" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A69" t="s">
+        <v>134</v>
+      </c>
+      <c r="B69">
+        <v>24</v>
+      </c>
+      <c r="C69" t="s">
+        <v>68</v>
+      </c>
+      <c r="D69" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="I47:J47"/>
-    <mergeCell ref="I52:J52"/>
-    <mergeCell ref="I57:J57"/>
+    <mergeCell ref="I53:J53"/>
+    <mergeCell ref="I58:J58"/>
+    <mergeCell ref="I63:J63"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D2:E33 F2:F25 G12">
-    <cfRule type="containsText" dxfId="14" priority="12" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="16" priority="13" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G38:G39">
-    <cfRule type="containsText" dxfId="11" priority="11" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",G38)))</formula>
+  <conditionalFormatting sqref="G44:G45">
+    <cfRule type="containsText" dxfId="13" priority="12" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",G44)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D40:D48">
-    <cfRule type="containsText" dxfId="9" priority="10" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",D40)))</formula>
+  <conditionalFormatting sqref="D46:D54">
+    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",D46)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D49:D55">
-    <cfRule type="containsText" dxfId="8" priority="9" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",D49)))</formula>
+  <conditionalFormatting sqref="D55:D61">
+    <cfRule type="containsText" dxfId="11" priority="10" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",D55)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D56:D66">
-    <cfRule type="containsText" dxfId="7" priority="8" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",D56)))</formula>
+  <conditionalFormatting sqref="D62:D72">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",D62)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="9" priority="8" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",G3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="8" priority="7" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",G4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:G6">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="6" priority="5" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",G5)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G8">
-    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="5" priority="4" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",G8)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G9">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",G9)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",G10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D38:E43">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",G10)))</formula>
+      <formula>NOT(ISERROR(SEARCH("N",D38)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3041,7 +3223,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <conditionalFormatting sqref="D2:E200 F23:F33 G23:G25 F12">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D2)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3053,11 +3235,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1375D86A-AC32-1C40-AB96-8DC0895D6135}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E23"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="11.5" customWidth="1"/>
+    <col min="3" max="3" width="26.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -3097,7 +3281,7 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F2" t="s">
         <v>110</v>
@@ -3117,7 +3301,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F3" t="s">
         <v>110</v>
@@ -3137,7 +3321,7 @@
         <v>6</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F4" t="s">
         <v>110</v>
@@ -3157,7 +3341,7 @@
         <v>6</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F5" t="s">
         <v>110</v>
@@ -3177,7 +3361,7 @@
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F6" t="s">
         <v>110</v>
@@ -3197,7 +3381,7 @@
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F7" t="s">
         <v>110</v>
@@ -3217,7 +3401,7 @@
         <v>6</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F8" t="s">
         <v>110</v>
@@ -3237,7 +3421,7 @@
         <v>6</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F9" t="s">
         <v>110</v>
@@ -3257,7 +3441,7 @@
         <v>6</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
         <v>110</v>
@@ -3277,7 +3461,7 @@
         <v>6</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F11" t="s">
         <v>110</v>
@@ -3297,7 +3481,7 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F12" t="s">
         <v>110</v>
@@ -3317,7 +3501,7 @@
         <v>6</v>
       </c>
       <c r="E13" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F13" t="s">
         <v>110</v>
@@ -3337,7 +3521,7 @@
         <v>6</v>
       </c>
       <c r="E14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
         <v>110</v>
@@ -3357,7 +3541,7 @@
         <v>6</v>
       </c>
       <c r="E15" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
         <v>110</v>
@@ -3377,7 +3561,7 @@
         <v>6</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F16" t="s">
         <v>110</v>
@@ -3397,7 +3581,7 @@
         <v>6</v>
       </c>
       <c r="E17" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F17" t="s">
         <v>110</v>
@@ -3417,7 +3601,7 @@
         <v>6</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F18" t="s">
         <v>110</v>
@@ -3437,7 +3621,7 @@
         <v>6</v>
       </c>
       <c r="E19" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F19" t="s">
         <v>110</v>
@@ -3457,7 +3641,7 @@
         <v>6</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F20" t="s">
         <v>110</v>
@@ -3477,7 +3661,7 @@
         <v>6</v>
       </c>
       <c r="E21" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F21" t="s">
         <v>110</v>
@@ -3497,7 +3681,7 @@
         <v>6</v>
       </c>
       <c r="E22" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F22" t="s">
         <v>110</v>
@@ -3517,7 +3701,7 @@
         <v>6</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F23" t="s">
         <v>110</v>
@@ -3525,8 +3709,8 @@
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="D2:E33 F2:F23">
-    <cfRule type="containsText" dxfId="10" priority="1" operator="containsText" text="N">
+  <conditionalFormatting sqref="F2:F23 D2:E33">
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",D2)))</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Variant caller jumpy depths bug fix
</commit_message>
<xml_diff>
--- a/data/Consensus_Data/Libraries_informatics_progress_sheet.xlsx
+++ b/data/Consensus_Data/Libraries_informatics_progress_sheet.xlsx
@@ -10,7 +10,7 @@
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="68" documentId="8_{A53EAE12-F6DD-E840-89F1-5D6C4362DC88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{878594EE-211F-AB42-AB82-8FE1D274633C}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{56B4F61F-FF81-5047-AAC1-D1034B21E8E5}"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="29920" windowHeight="18680" activeTab="2" xr2:uid="{56B4F61F-FF81-5047-AAC1-D1034B21E8E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Lane28" sheetId="2" r:id="rId1"/>
@@ -1010,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14F2D043-530F-0C4F-9959-B35E9CE1CB91}">
   <dimension ref="A1:J69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="200" workbookViewId="0">
+    <sheetView topLeftCell="A31" zoomScale="200" workbookViewId="0">
       <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
@@ -3235,8 +3235,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1375D86A-AC32-1C40-AB96-8DC0895D6135}">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2:E23"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>